<commit_message>
Modified test 3.6.0. Added page object.
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -1535,7 +1535,6 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
-  <si/>
   <si>
     <t>Проверка раздела News</t>
   </si>
@@ -2283,6 +2282,15 @@
   <si>
     <r>
       <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>Доделать. В процессе.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <rFont val="Courier"/>
         <sz val="11"/>
       </rPr>
@@ -2554,6 +2562,9 @@
   </si>
   <si>
     <t>Переход в раздел About успешный</t>
+  </si>
+  <si>
+    <t>Доделать. В процессе.</t>
   </si>
   <si>
     <t>Перейти по ссылке в Privace Policy</t>
@@ -3158,7 +3169,7 @@
   <cellStyleXfs count="1">
     <xf applyFont="true" borderId="0" fillId="0" fontId="1" quotePrefix="false"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="209">
     <xf applyFont="true" borderId="0" fillId="0" fontId="1" quotePrefix="false"/>
     <xf applyAlignment="true" applyFill="true" applyFont="true" borderId="0" fillId="2" fontId="1" quotePrefix="false">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
@@ -3612,7 +3623,7 @@
     <xf applyBorder="true" applyFont="true" borderId="2" fillId="0" fontId="0" quotePrefix="false"/>
     <xf applyBorder="true" applyFont="true" borderId="4" fillId="0" fontId="2" quotePrefix="false"/>
     <xf applyBorder="true" applyFont="true" borderId="5" fillId="0" fontId="2" quotePrefix="false"/>
-    <xf applyBorder="true" applyFont="true" borderId="6" fillId="0" fontId="2" quotePrefix="false"/>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="6" fillId="20" fontId="1" quotePrefix="false"/>
     <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" borderId="7" fillId="13" fontId="3" quotePrefix="false">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
@@ -3660,6 +3671,9 @@
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" borderId="33" fillId="0" fontId="1" quotePrefix="false">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" borderId="6" fillId="20" fontId="1" quotePrefix="false">
+      <alignment wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" borderId="9" fillId="0" fontId="1" quotePrefix="false">
       <alignment horizontal="right" vertical="center"/>
@@ -6684,9 +6698,7 @@
       <c r="G131" s="135" t="s">
         <v>245</v>
       </c>
-      <c r="H131" s="136" t="s">
-        <v>255</v>
-      </c>
+      <c r="H131" s="136" t="n"/>
       <c r="I131" s="0" t="s">
         <v>22</v>
       </c>
@@ -6726,9 +6738,7 @@
       <c r="G133" s="138" t="s">
         <v>245</v>
       </c>
-      <c r="H133" s="139" t="s">
-        <v>255</v>
-      </c>
+      <c r="H133" s="139" t="n"/>
       <c r="I133" s="29" t="s">
         <v>22</v>
       </c>
@@ -6741,7 +6751,7 @@
         <v>19</v>
       </c>
       <c r="B134" s="140" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C134" s="35" t="n"/>
       <c r="D134" s="35" t="n"/>
@@ -6749,10 +6759,10 @@
         <v>65</v>
       </c>
       <c r="F134" s="37" t="s">
+        <v>256</v>
+      </c>
+      <c r="G134" s="38" t="s">
         <v>257</v>
-      </c>
-      <c r="G134" s="38" t="s">
-        <v>258</v>
       </c>
       <c r="H134" s="55" t="n"/>
       <c r="I134" s="12" t="s">
@@ -6769,14 +6779,14 @@
       <c r="D135" s="0" t="n"/>
       <c r="E135" s="65" t="s"/>
       <c r="F135" s="142" t="s">
+        <v>258</v>
+      </c>
+      <c r="G135" s="143" t="s">
         <v>259</v>
-      </c>
-      <c r="G135" s="143" t="s">
-        <v>260</v>
       </c>
       <c r="H135" s="144" t="n"/>
       <c r="I135" s="145" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J135" s="21" t="s">
         <v>15</v>
@@ -6789,10 +6799,10 @@
       <c r="D136" s="0" t="n"/>
       <c r="E136" s="65" t="s"/>
       <c r="F136" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="G136" s="21" t="s">
         <v>262</v>
-      </c>
-      <c r="G136" s="21" t="s">
-        <v>263</v>
       </c>
       <c r="H136" s="43" t="n"/>
       <c r="I136" s="0" t="s">
@@ -6809,10 +6819,10 @@
       <c r="D137" s="0" t="n"/>
       <c r="E137" s="65" t="s"/>
       <c r="F137" s="146" t="s">
+        <v>263</v>
+      </c>
+      <c r="G137" s="147" t="s">
         <v>264</v>
-      </c>
-      <c r="G137" s="147" t="s">
-        <v>265</v>
       </c>
       <c r="H137" s="43" t="n"/>
       <c r="I137" s="0" t="s">
@@ -6829,10 +6839,10 @@
       <c r="D138" s="58" t="n"/>
       <c r="E138" s="65" t="s"/>
       <c r="F138" s="148" t="s">
+        <v>265</v>
+      </c>
+      <c r="G138" s="149" t="s">
         <v>266</v>
-      </c>
-      <c r="G138" s="149" t="s">
-        <v>267</v>
       </c>
       <c r="H138" s="59" t="n"/>
       <c r="I138" s="29" t="s">
@@ -6847,7 +6857,7 @@
         <v>20</v>
       </c>
       <c r="B139" s="150" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C139" s="12" t="n"/>
       <c r="D139" s="12" t="n"/>
@@ -6855,10 +6865,10 @@
         <v>65</v>
       </c>
       <c r="F139" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G139" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H139" s="16" t="n"/>
       <c r="I139" s="151" t="s">
@@ -6875,10 +6885,10 @@
       <c r="D140" s="0" t="n"/>
       <c r="E140" s="70" t="s"/>
       <c r="F140" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="G140" s="21" t="s">
         <v>270</v>
-      </c>
-      <c r="G140" s="21" t="s">
-        <v>271</v>
       </c>
       <c r="H140" s="22" t="n"/>
       <c r="I140" s="152" t="s">
@@ -6895,10 +6905,10 @@
       <c r="D141" s="0" t="n"/>
       <c r="E141" s="70" t="s"/>
       <c r="F141" s="153" t="s">
+        <v>271</v>
+      </c>
+      <c r="G141" s="125" t="s">
         <v>272</v>
-      </c>
-      <c r="G141" s="125" t="s">
-        <v>273</v>
       </c>
       <c r="H141" s="83" t="s">
         <v>134</v>
@@ -6917,14 +6927,14 @@
       <c r="D142" s="0" t="n"/>
       <c r="E142" s="70" t="s"/>
       <c r="F142" s="155" t="s">
+        <v>273</v>
+      </c>
+      <c r="G142" s="143" t="s">
         <v>274</v>
-      </c>
-      <c r="G142" s="143" t="s">
-        <v>275</v>
       </c>
       <c r="H142" s="156" t="n"/>
       <c r="I142" s="145" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J142" s="21" t="s">
         <v>15</v>
@@ -6937,14 +6947,14 @@
       <c r="D143" s="0" t="n"/>
       <c r="E143" s="70" t="s"/>
       <c r="F143" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="G143" s="143" t="s">
         <v>277</v>
-      </c>
-      <c r="G143" s="143" t="s">
-        <v>278</v>
       </c>
       <c r="H143" s="156" t="n"/>
       <c r="I143" s="145" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J143" s="21" t="s">
         <v>15</v>
@@ -6957,10 +6967,10 @@
       <c r="D144" s="0" t="n"/>
       <c r="E144" s="70" t="s"/>
       <c r="F144" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="G144" s="24" t="s">
         <v>279</v>
-      </c>
-      <c r="G144" s="24" t="s">
-        <v>280</v>
       </c>
       <c r="H144" s="22" t="n"/>
       <c r="I144" s="152" t="s">
@@ -6977,10 +6987,10 @@
       <c r="D145" s="29" t="n"/>
       <c r="E145" s="70" t="s"/>
       <c r="F145" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="G145" s="32" t="s">
         <v>281</v>
-      </c>
-      <c r="G145" s="32" t="s">
-        <v>282</v>
       </c>
       <c r="H145" s="33" t="n"/>
       <c r="I145" s="157" t="s">
@@ -6995,7 +7005,7 @@
         <v>21</v>
       </c>
       <c r="B146" s="150" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C146" s="12" t="n"/>
       <c r="D146" s="12" t="n"/>
@@ -7003,10 +7013,10 @@
         <v>65</v>
       </c>
       <c r="F146" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="G146" s="73" t="s">
         <v>284</v>
-      </c>
-      <c r="G146" s="73" t="s">
-        <v>285</v>
       </c>
       <c r="H146" s="16" t="n"/>
       <c r="I146" s="151" t="s">
@@ -7023,10 +7033,10 @@
       <c r="D147" s="0" t="n"/>
       <c r="E147" s="70" t="s"/>
       <c r="F147" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="G147" s="21" t="s">
         <v>286</v>
-      </c>
-      <c r="G147" s="21" t="s">
-        <v>287</v>
       </c>
       <c r="H147" s="22" t="n"/>
       <c r="I147" s="152" t="s">
@@ -7043,10 +7053,10 @@
       <c r="D148" s="0" t="n"/>
       <c r="E148" s="70" t="s"/>
       <c r="F148" s="146" t="s">
+        <v>287</v>
+      </c>
+      <c r="G148" s="158" t="s">
         <v>288</v>
-      </c>
-      <c r="G148" s="158" t="s">
-        <v>289</v>
       </c>
       <c r="H148" s="22" t="n"/>
       <c r="I148" s="152" t="s">
@@ -7063,10 +7073,10 @@
       <c r="D149" s="0" t="n"/>
       <c r="E149" s="70" t="s"/>
       <c r="F149" s="146" t="s">
+        <v>289</v>
+      </c>
+      <c r="G149" s="158" t="s">
         <v>290</v>
-      </c>
-      <c r="G149" s="158" t="s">
-        <v>291</v>
       </c>
       <c r="H149" s="22" t="n"/>
       <c r="I149" s="152" t="s">
@@ -7083,10 +7093,10 @@
       <c r="D150" s="0" t="n"/>
       <c r="E150" s="70" t="s"/>
       <c r="F150" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="G150" s="21" t="s">
         <v>292</v>
-      </c>
-      <c r="G150" s="21" t="s">
-        <v>293</v>
       </c>
       <c r="H150" s="22" t="n"/>
       <c r="I150" s="152" t="s">
@@ -7103,14 +7113,14 @@
       <c r="D151" s="0" t="n"/>
       <c r="E151" s="70" t="s"/>
       <c r="F151" s="146" t="s">
+        <v>293</v>
+      </c>
+      <c r="G151" s="159" t="s">
         <v>294</v>
-      </c>
-      <c r="G151" s="159" t="s">
-        <v>295</v>
       </c>
       <c r="H151" s="156" t="n"/>
       <c r="I151" s="145" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J151" s="21" t="s">
         <v>15</v>
@@ -7123,14 +7133,14 @@
       <c r="D152" s="29" t="n"/>
       <c r="E152" s="70" t="s"/>
       <c r="F152" s="160" t="s">
+        <v>296</v>
+      </c>
+      <c r="G152" s="161" t="s">
         <v>297</v>
-      </c>
-      <c r="G152" s="161" t="s">
-        <v>298</v>
       </c>
       <c r="H152" s="162" t="n"/>
       <c r="I152" s="163" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J152" s="32" t="s">
         <v>15</v>
@@ -7141,7 +7151,7 @@
         <v>22</v>
       </c>
       <c r="B153" s="150" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C153" s="12" t="n"/>
       <c r="D153" s="12" t="n"/>
@@ -7149,10 +7159,10 @@
         <v>65</v>
       </c>
       <c r="F153" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="G153" s="73" t="s">
         <v>300</v>
-      </c>
-      <c r="G153" s="73" t="s">
-        <v>301</v>
       </c>
       <c r="H153" s="16" t="n"/>
       <c r="I153" s="151" t="s">
@@ -7169,10 +7179,10 @@
       <c r="D154" s="0" t="n"/>
       <c r="E154" s="70" t="s"/>
       <c r="F154" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="G154" s="21" t="s">
         <v>302</v>
-      </c>
-      <c r="G154" s="21" t="s">
-        <v>303</v>
       </c>
       <c r="H154" s="22" t="n"/>
       <c r="I154" s="152" t="s">
@@ -7189,10 +7199,10 @@
       <c r="D155" s="0" t="n"/>
       <c r="E155" s="70" t="s"/>
       <c r="F155" s="81" t="s">
+        <v>303</v>
+      </c>
+      <c r="G155" s="125" t="s">
         <v>304</v>
-      </c>
-      <c r="G155" s="125" t="s">
-        <v>305</v>
       </c>
       <c r="H155" s="83" t="s">
         <v>134</v>
@@ -7211,14 +7221,14 @@
       <c r="D156" s="0" t="n"/>
       <c r="E156" s="70" t="s"/>
       <c r="F156" s="155" t="s">
+        <v>273</v>
+      </c>
+      <c r="G156" s="143" t="s">
         <v>274</v>
-      </c>
-      <c r="G156" s="143" t="s">
-        <v>275</v>
       </c>
       <c r="H156" s="156" t="n"/>
       <c r="I156" s="145" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J156" s="21" t="s">
         <v>15</v>
@@ -7231,14 +7241,14 @@
       <c r="D157" s="0" t="n"/>
       <c r="E157" s="70" t="s"/>
       <c r="F157" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="G157" s="143" t="s">
         <v>277</v>
-      </c>
-      <c r="G157" s="143" t="s">
-        <v>278</v>
       </c>
       <c r="H157" s="156" t="n"/>
       <c r="I157" s="145" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J157" s="21" t="s">
         <v>15</v>
@@ -7251,10 +7261,10 @@
       <c r="D158" s="0" t="n"/>
       <c r="E158" s="70" t="s"/>
       <c r="F158" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="G158" s="21" t="s">
         <v>306</v>
-      </c>
-      <c r="G158" s="21" t="s">
-        <v>307</v>
       </c>
       <c r="H158" s="22" t="n"/>
       <c r="I158" s="152" t="s">
@@ -7271,10 +7281,10 @@
       <c r="D159" s="0" t="n"/>
       <c r="E159" s="70" t="s"/>
       <c r="F159" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="G159" s="21" t="s">
         <v>308</v>
-      </c>
-      <c r="G159" s="21" t="s">
-        <v>309</v>
       </c>
       <c r="H159" s="22" t="n"/>
       <c r="I159" s="152" t="s">
@@ -7294,7 +7304,7 @@
         <v>144</v>
       </c>
       <c r="G160" s="21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H160" s="22" t="n"/>
       <c r="I160" s="152" t="s">
@@ -7311,10 +7321,10 @@
       <c r="D161" s="29" t="n"/>
       <c r="E161" s="70" t="s"/>
       <c r="F161" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="G161" s="32" t="s">
         <v>311</v>
-      </c>
-      <c r="G161" s="32" t="s">
-        <v>312</v>
       </c>
       <c r="H161" s="33" t="n"/>
       <c r="I161" s="157" t="s">
@@ -7329,7 +7339,7 @@
         <v>23</v>
       </c>
       <c r="B162" s="150" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C162" s="12" t="n"/>
       <c r="D162" s="12" t="n"/>
@@ -7337,10 +7347,10 @@
         <v>65</v>
       </c>
       <c r="F162" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G162" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H162" s="16" t="n"/>
       <c r="I162" s="12" t="s">
@@ -7357,10 +7367,10 @@
       <c r="D163" s="0" t="n"/>
       <c r="E163" s="70" t="s"/>
       <c r="F163" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="G163" s="21" t="s">
         <v>302</v>
-      </c>
-      <c r="G163" s="21" t="s">
-        <v>303</v>
       </c>
       <c r="H163" s="22" t="n"/>
       <c r="I163" s="0" t="s">
@@ -7377,10 +7387,10 @@
       <c r="D164" s="0" t="n"/>
       <c r="E164" s="70" t="s"/>
       <c r="F164" s="81" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G164" s="125" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H164" s="83" t="s">
         <v>134</v>
@@ -7399,10 +7409,10 @@
       <c r="D165" s="0" t="n"/>
       <c r="E165" s="70" t="s"/>
       <c r="F165" s="146" t="s">
+        <v>315</v>
+      </c>
+      <c r="G165" s="147" t="s">
         <v>316</v>
-      </c>
-      <c r="G165" s="147" t="s">
-        <v>317</v>
       </c>
       <c r="H165" s="22" t="n"/>
       <c r="I165" s="0" t="s">
@@ -7419,14 +7429,14 @@
       <c r="D166" s="0" t="n"/>
       <c r="E166" s="70" t="s"/>
       <c r="F166" s="23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G166" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H166" s="22" t="n"/>
       <c r="I166" s="0" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J166" s="21" t="s">
         <v>15</v>
@@ -7442,11 +7452,11 @@
         <v>137</v>
       </c>
       <c r="G167" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H167" s="22" t="n"/>
       <c r="I167" s="152" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J167" s="21" t="s">
         <v>15</v>
@@ -7459,13 +7469,13 @@
       <c r="D168" s="0" t="n"/>
       <c r="E168" s="70" t="s"/>
       <c r="F168" s="146" t="s">
+        <v>319</v>
+      </c>
+      <c r="G168" s="147" t="s">
         <v>320</v>
       </c>
-      <c r="G168" s="147" t="s">
+      <c r="H168" s="164" t="s">
         <v>321</v>
-      </c>
-      <c r="H168" s="164" t="s">
-        <v>322</v>
       </c>
       <c r="I168" s="0" t="s">
         <v>22</v>
@@ -7481,19 +7491,19 @@
       <c r="D169" s="0" t="n"/>
       <c r="E169" s="70" t="s"/>
       <c r="F169" s="165" t="s">
+        <v>322</v>
+      </c>
+      <c r="G169" s="159" t="s">
         <v>323</v>
       </c>
-      <c r="G169" s="159" t="s">
+      <c r="H169" s="166" t="s">
         <v>324</v>
       </c>
-      <c r="H169" s="166" t="s">
+      <c r="I169" s="152" t="s">
         <v>325</v>
       </c>
-      <c r="I169" s="152" t="s">
+      <c r="J169" s="21" t="s">
         <v>326</v>
-      </c>
-      <c r="J169" s="21" t="s">
-        <v>327</v>
       </c>
     </row>
     <row outlineLevel="0" r="170">
@@ -7506,7 +7516,7 @@
         <v>126</v>
       </c>
       <c r="G170" s="24" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H170" s="22" t="n"/>
       <c r="I170" s="0" t="s">
@@ -7523,10 +7533,10 @@
       <c r="D171" s="29" t="n"/>
       <c r="E171" s="70" t="s"/>
       <c r="F171" s="71" t="s">
+        <v>328</v>
+      </c>
+      <c r="G171" s="32" t="s">
         <v>329</v>
-      </c>
-      <c r="G171" s="32" t="s">
-        <v>330</v>
       </c>
       <c r="H171" s="33" t="n"/>
       <c r="I171" s="29" t="s">
@@ -7541,7 +7551,7 @@
         <v>24</v>
       </c>
       <c r="B172" s="150" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C172" s="12" t="n"/>
       <c r="D172" s="12" t="n"/>
@@ -7549,10 +7559,10 @@
         <v>65</v>
       </c>
       <c r="F172" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="G172" s="15" t="s">
         <v>332</v>
-      </c>
-      <c r="G172" s="15" t="s">
-        <v>333</v>
       </c>
       <c r="H172" s="16" t="n"/>
       <c r="I172" s="151" t="s">
@@ -7569,10 +7579,10 @@
       <c r="D173" s="0" t="n"/>
       <c r="E173" s="70" t="s"/>
       <c r="F173" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="G173" s="21" t="s">
         <v>334</v>
-      </c>
-      <c r="G173" s="21" t="s">
-        <v>335</v>
       </c>
       <c r="H173" s="22" t="n"/>
       <c r="I173" s="152" t="s">
@@ -7589,13 +7599,13 @@
       <c r="D174" s="0" t="n"/>
       <c r="E174" s="70" t="s"/>
       <c r="F174" s="81" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G174" s="125" t="s">
         <v>145</v>
       </c>
       <c r="H174" s="83" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I174" s="152" t="s">
         <v>22</v>
@@ -7611,10 +7621,10 @@
       <c r="D175" s="29" t="n"/>
       <c r="E175" s="70" t="s"/>
       <c r="F175" s="167" t="s">
+        <v>337</v>
+      </c>
+      <c r="G175" s="168" t="s">
         <v>338</v>
-      </c>
-      <c r="G175" s="168" t="s">
-        <v>339</v>
       </c>
       <c r="H175" s="169" t="s">
         <v>134</v>
@@ -7631,7 +7641,7 @@
         <v>25</v>
       </c>
       <c r="B176" s="150" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C176" s="12" t="n"/>
       <c r="D176" s="12" t="n"/>
@@ -7639,10 +7649,10 @@
         <v>65</v>
       </c>
       <c r="F176" s="37" t="s">
+        <v>340</v>
+      </c>
+      <c r="G176" s="126" t="s">
         <v>341</v>
-      </c>
-      <c r="G176" s="126" t="s">
-        <v>342</v>
       </c>
       <c r="H176" s="55" t="n"/>
       <c r="I176" s="55" t="s">
@@ -7659,10 +7669,10 @@
       <c r="D177" s="0" t="n"/>
       <c r="E177" s="171" t="s"/>
       <c r="F177" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="G177" s="45" t="s">
         <v>302</v>
-      </c>
-      <c r="G177" s="45" t="s">
-        <v>303</v>
       </c>
       <c r="H177" s="43" t="n"/>
       <c r="I177" s="43" t="s">
@@ -7679,10 +7689,10 @@
       <c r="D178" s="0" t="n"/>
       <c r="E178" s="171" t="s"/>
       <c r="F178" s="46" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G178" s="45" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H178" s="43" t="n"/>
       <c r="I178" s="43" t="s">
@@ -7699,10 +7709,10 @@
       <c r="D179" s="0" t="n"/>
       <c r="E179" s="171" t="s"/>
       <c r="F179" s="93" t="s">
+        <v>315</v>
+      </c>
+      <c r="G179" s="172" t="s">
         <v>316</v>
-      </c>
-      <c r="G179" s="172" t="s">
-        <v>317</v>
       </c>
       <c r="H179" s="43" t="n"/>
       <c r="I179" s="43" t="s">
@@ -7719,14 +7729,14 @@
       <c r="D180" s="0" t="n"/>
       <c r="E180" s="171" t="s"/>
       <c r="F180" s="173" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G180" s="174" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H180" s="144" t="n"/>
       <c r="I180" s="144" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J180" s="47" t="s">
         <v>15</v>
@@ -7742,11 +7752,11 @@
         <v>137</v>
       </c>
       <c r="G181" s="174" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H181" s="144" t="n"/>
       <c r="I181" s="144" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J181" s="47" t="s">
         <v>15</v>
@@ -7759,10 +7769,10 @@
       <c r="D182" s="0" t="n"/>
       <c r="E182" s="171" t="s"/>
       <c r="F182" s="93" t="s">
+        <v>319</v>
+      </c>
+      <c r="G182" s="172" t="s">
         <v>320</v>
-      </c>
-      <c r="G182" s="172" t="s">
-        <v>321</v>
       </c>
       <c r="H182" s="43" t="n"/>
       <c r="I182" s="43" t="s">
@@ -7779,10 +7789,10 @@
       <c r="D183" s="0" t="n"/>
       <c r="E183" s="171" t="s"/>
       <c r="F183" s="93" t="s">
+        <v>344</v>
+      </c>
+      <c r="G183" s="172" t="s">
         <v>345</v>
-      </c>
-      <c r="G183" s="172" t="s">
-        <v>346</v>
       </c>
       <c r="H183" s="43" t="n"/>
       <c r="I183" s="43" t="s">
@@ -7802,7 +7812,7 @@
         <v>126</v>
       </c>
       <c r="G184" s="42" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H184" s="43" t="n"/>
       <c r="I184" s="43" t="s">
@@ -7819,10 +7829,10 @@
       <c r="D185" s="29" t="n"/>
       <c r="E185" s="171" t="s"/>
       <c r="F185" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="G185" s="45" t="s">
         <v>329</v>
-      </c>
-      <c r="G185" s="45" t="s">
-        <v>330</v>
       </c>
       <c r="H185" s="43" t="n"/>
       <c r="I185" s="43" t="s">
@@ -7839,10 +7849,10 @@
       <c r="D186" s="29" t="s"/>
       <c r="E186" s="171" t="s"/>
       <c r="F186" s="66" t="s">
+        <v>346</v>
+      </c>
+      <c r="G186" s="50" t="s">
         <v>347</v>
-      </c>
-      <c r="G186" s="50" t="s">
-        <v>348</v>
       </c>
       <c r="H186" s="59" t="n"/>
       <c r="I186" s="59" t="s">
@@ -7855,18 +7865,18 @@
         <v>26</v>
       </c>
       <c r="B187" s="150" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C187" s="12" t="n"/>
       <c r="D187" s="12" t="n"/>
       <c r="E187" s="68" t="s">
+        <v>349</v>
+      </c>
+      <c r="F187" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="F187" s="14" t="s">
-        <v>351</v>
-      </c>
       <c r="G187" s="15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H187" s="176" t="n"/>
       <c r="I187" s="12" t="s">
@@ -7883,13 +7893,13 @@
       <c r="D188" s="0" t="n"/>
       <c r="E188" s="70" t="s"/>
       <c r="F188" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="G188" s="21" t="s">
         <v>352</v>
       </c>
-      <c r="G188" s="21" t="s">
+      <c r="H188" s="177" t="s">
         <v>353</v>
-      </c>
-      <c r="H188" s="177" t="s">
-        <v>354</v>
       </c>
       <c r="I188" s="0" t="s">
         <v>22</v>
@@ -7905,13 +7915,13 @@
       <c r="D189" s="0" t="n"/>
       <c r="E189" s="70" t="s"/>
       <c r="F189" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="G189" s="21" t="s">
         <v>355</v>
       </c>
-      <c r="G189" s="21" t="s">
+      <c r="H189" s="86" t="s">
         <v>356</v>
-      </c>
-      <c r="H189" s="86" t="s">
-        <v>357</v>
       </c>
       <c r="I189" s="0" t="s">
         <v>22</v>
@@ -7927,13 +7937,13 @@
       <c r="D190" s="29" t="n"/>
       <c r="E190" s="70" t="s"/>
       <c r="F190" s="71" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G190" s="32" t="s">
+        <v>355</v>
+      </c>
+      <c r="H190" s="72" t="s">
         <v>356</v>
-      </c>
-      <c r="H190" s="72" t="s">
-        <v>357</v>
       </c>
       <c r="I190" s="29" t="s">
         <v>22</v>
@@ -7947,7 +7957,7 @@
         <v>27</v>
       </c>
       <c r="B191" s="178" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C191" s="179" t="n"/>
       <c r="D191" s="12" t="s"/>
@@ -7955,13 +7965,13 @@
         <v>65</v>
       </c>
       <c r="F191" s="37" t="s">
+        <v>359</v>
+      </c>
+      <c r="G191" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="H191" s="180" t="s">
         <v>360</v>
-      </c>
-      <c r="G191" s="38" t="s">
-        <v>356</v>
-      </c>
-      <c r="H191" s="180" t="s">
-        <v>361</v>
       </c>
       <c r="I191" s="63" t="s">
         <v>22</v>
@@ -7975,13 +7985,13 @@
       <c r="D192" s="182" t="s"/>
       <c r="E192" s="171" t="s"/>
       <c r="F192" s="46" t="s">
+        <v>354</v>
+      </c>
+      <c r="G192" s="45" t="s">
         <v>355</v>
       </c>
-      <c r="G192" s="45" t="s">
-        <v>356</v>
-      </c>
       <c r="H192" s="47" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I192" s="41" t="s">
         <v>22</v>
@@ -7997,13 +8007,13 @@
       <c r="D193" s="29" t="s"/>
       <c r="E193" s="171" t="s"/>
       <c r="F193" s="66" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G193" s="50" t="s">
+        <v>355</v>
+      </c>
+      <c r="H193" s="96" t="s">
         <v>356</v>
-      </c>
-      <c r="H193" s="96" t="s">
-        <v>357</v>
       </c>
       <c r="I193" s="52" t="s">
         <v>22</v>
@@ -8017,7 +8027,7 @@
         <v>28</v>
       </c>
       <c r="B194" s="150" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C194" s="12" t="n"/>
       <c r="D194" s="12" t="n"/>
@@ -8025,10 +8035,10 @@
         <v>65</v>
       </c>
       <c r="F194" s="183" t="s">
+        <v>363</v>
+      </c>
+      <c r="G194" s="184" t="s">
         <v>364</v>
-      </c>
-      <c r="G194" s="184" t="s">
-        <v>365</v>
       </c>
       <c r="H194" s="16" t="n"/>
       <c r="I194" s="12" t="s">
@@ -8045,10 +8055,10 @@
       <c r="D195" s="0" t="n"/>
       <c r="E195" s="70" t="s"/>
       <c r="F195" s="20" t="s">
+        <v>365</v>
+      </c>
+      <c r="G195" s="21" t="s">
         <v>366</v>
-      </c>
-      <c r="G195" s="21" t="s">
-        <v>367</v>
       </c>
       <c r="H195" s="22" t="n"/>
       <c r="I195" s="0" t="s">
@@ -8065,10 +8075,10 @@
       <c r="D196" s="29" t="n"/>
       <c r="E196" s="70" t="s"/>
       <c r="F196" s="71" t="s">
+        <v>367</v>
+      </c>
+      <c r="G196" s="32" t="s">
         <v>368</v>
-      </c>
-      <c r="G196" s="32" t="s">
-        <v>369</v>
       </c>
       <c r="H196" s="33" t="n"/>
       <c r="I196" s="29" t="s">
@@ -8083,7 +8093,7 @@
         <v>29</v>
       </c>
       <c r="B197" s="185" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C197" s="186" t="n"/>
       <c r="D197" s="186" t="n"/>
@@ -8091,12 +8101,14 @@
         <v>65</v>
       </c>
       <c r="F197" s="187" t="s">
+        <v>370</v>
+      </c>
+      <c r="G197" s="188" t="s">
         <v>371</v>
       </c>
-      <c r="G197" s="188" t="s">
+      <c r="H197" s="189" t="s">
         <v>372</v>
       </c>
-      <c r="H197" s="189" t="n"/>
       <c r="I197" s="12" t="n"/>
       <c r="J197" s="15" t="s">
         <v>15</v>
@@ -8250,7 +8262,9 @@
       <c r="G205" s="15" t="s">
         <v>389</v>
       </c>
-      <c r="H205" s="16" t="n"/>
+      <c r="H205" s="189" t="s">
+        <v>372</v>
+      </c>
       <c r="I205" s="12" t="n"/>
       <c r="J205" s="15" t="s">
         <v>15</v>
@@ -8382,7 +8396,9 @@
       <c r="G212" s="73" t="s">
         <v>403</v>
       </c>
-      <c r="H212" s="16" t="n"/>
+      <c r="H212" s="189" t="s">
+        <v>372</v>
+      </c>
       <c r="I212" s="12" t="n"/>
       <c r="J212" s="15" t="s">
         <v>15</v>
@@ -8514,7 +8530,9 @@
       <c r="G219" s="73" t="s">
         <v>403</v>
       </c>
-      <c r="H219" s="16" t="n"/>
+      <c r="H219" s="189" t="s">
+        <v>372</v>
+      </c>
       <c r="I219" s="12" t="n"/>
       <c r="J219" s="15" t="s">
         <v>15</v>
@@ -8608,23 +8626,25 @@
       <c r="G224" s="73" t="s">
         <v>419</v>
       </c>
-      <c r="H224" s="176" t="n"/>
+      <c r="H224" s="206" t="s">
+        <v>420</v>
+      </c>
       <c r="I224" s="14" t="n"/>
       <c r="J224" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row outlineLevel="0" r="225">
-      <c r="A225" s="206" t="s"/>
+      <c r="A225" s="207" t="s"/>
       <c r="B225" s="17" t="s"/>
       <c r="C225" s="0" t="n"/>
       <c r="D225" s="0" t="n"/>
       <c r="E225" s="24" t="n"/>
       <c r="F225" s="23" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G225" s="21" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="H225" s="86" t="n"/>
       <c r="I225" s="20" t="n"/>
@@ -8633,16 +8653,16 @@
       </c>
     </row>
     <row outlineLevel="0" r="226">
-      <c r="A226" s="206" t="s"/>
+      <c r="A226" s="207" t="s"/>
       <c r="B226" s="17" t="s"/>
       <c r="C226" s="0" t="n"/>
       <c r="D226" s="0" t="n"/>
       <c r="E226" s="24" t="n"/>
       <c r="F226" s="23" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="G226" s="21" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="H226" s="86" t="n"/>
       <c r="I226" s="20" t="n"/>
@@ -8651,16 +8671,16 @@
       </c>
     </row>
     <row outlineLevel="0" r="227">
-      <c r="A227" s="207" t="s"/>
+      <c r="A227" s="208" t="s"/>
       <c r="B227" s="27" t="s"/>
       <c r="C227" s="29" t="n"/>
       <c r="D227" s="29" t="n"/>
       <c r="E227" s="75" t="n"/>
       <c r="F227" s="31" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G227" s="75" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H227" s="72" t="n"/>
       <c r="I227" s="71" t="n"/>
@@ -8669,108 +8689,108 @@
   </sheetData>
   <mergeCells count="103">
     <mergeCell ref="E2:E8"/>
-    <mergeCell ref="E9:E18"/>
-    <mergeCell ref="E219:E223"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="E153:E161"/>
     <mergeCell ref="E77:E81"/>
     <mergeCell ref="E162:E171"/>
     <mergeCell ref="E71:E76"/>
     <mergeCell ref="E146:E152"/>
     <mergeCell ref="E194:E196"/>
-    <mergeCell ref="E67:E70"/>
+    <mergeCell ref="E54:E66"/>
     <mergeCell ref="E33:E41"/>
     <mergeCell ref="E85:E103"/>
     <mergeCell ref="E205:E211"/>
-    <mergeCell ref="E139:E145"/>
+    <mergeCell ref="E127:E133"/>
     <mergeCell ref="B224:B227"/>
-    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="B191:B193"/>
+    <mergeCell ref="B162:B171"/>
+    <mergeCell ref="B9:B18"/>
+    <mergeCell ref="B104:B116"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="B139:B145"/>
     <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B187:B190"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B104:B116"/>
-    <mergeCell ref="B205:B211"/>
-    <mergeCell ref="B121:B126"/>
-    <mergeCell ref="B9:B18"/>
+    <mergeCell ref="B85:B103"/>
     <mergeCell ref="A9:A18"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A71:A76"/>
-    <mergeCell ref="A104:A116"/>
+    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="A191:A193"/>
+    <mergeCell ref="A172:A175"/>
+    <mergeCell ref="A146:A152"/>
+    <mergeCell ref="A134:A138"/>
     <mergeCell ref="A153:A161"/>
-    <mergeCell ref="A191:A193"/>
-    <mergeCell ref="A146:A152"/>
-    <mergeCell ref="A139:A145"/>
-    <mergeCell ref="A212:A218"/>
-    <mergeCell ref="A162:A171"/>
+    <mergeCell ref="A205:A211"/>
     <mergeCell ref="D185:D186"/>
-    <mergeCell ref="E191:E193"/>
     <mergeCell ref="E176:E186"/>
     <mergeCell ref="E187:E190"/>
+    <mergeCell ref="E191:E193"/>
     <mergeCell ref="C191:D193"/>
     <mergeCell ref="C185:C186"/>
+    <mergeCell ref="A46:A53"/>
+    <mergeCell ref="A162:A171"/>
+    <mergeCell ref="A187:A190"/>
+    <mergeCell ref="A194:A196"/>
+    <mergeCell ref="A219:A223"/>
+    <mergeCell ref="A176:A186"/>
+    <mergeCell ref="A197:A204"/>
+    <mergeCell ref="A104:A116"/>
+    <mergeCell ref="B219:B223"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B54:B66"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B33:B41"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B146:B152"/>
+    <mergeCell ref="B121:B126"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="B127:B133"/>
+    <mergeCell ref="B176:B186"/>
+    <mergeCell ref="B134:B138"/>
+    <mergeCell ref="B153:B161"/>
+    <mergeCell ref="B46:B53"/>
+    <mergeCell ref="B205:B211"/>
+    <mergeCell ref="B172:B175"/>
+    <mergeCell ref="A139:A145"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="A224:A227"/>
+    <mergeCell ref="A121:A126"/>
+    <mergeCell ref="A85:A103"/>
+    <mergeCell ref="A212:A218"/>
+    <mergeCell ref="A71:A76"/>
     <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A41"/>
-    <mergeCell ref="A187:A190"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A127:A133"/>
-    <mergeCell ref="A121:A126"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="B172:B175"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="B54:B66"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="B33:B41"/>
-    <mergeCell ref="B134:B138"/>
-    <mergeCell ref="B127:B133"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="B139:B145"/>
-    <mergeCell ref="B146:B152"/>
-    <mergeCell ref="B176:B186"/>
-    <mergeCell ref="B162:B171"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B197:B204"/>
-    <mergeCell ref="B212:B218"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A134:A138"/>
-    <mergeCell ref="A219:A223"/>
-    <mergeCell ref="A224:A227"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="A176:A186"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A77:A81"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="E9:E18"/>
+    <mergeCell ref="E172:E175"/>
+    <mergeCell ref="E212:E218"/>
+    <mergeCell ref="E121:E126"/>
+    <mergeCell ref="E104:E116"/>
+    <mergeCell ref="E46:E53"/>
+    <mergeCell ref="E219:E223"/>
     <mergeCell ref="E19:E21"/>
     <mergeCell ref="E30:E32"/>
-    <mergeCell ref="E172:E175"/>
-    <mergeCell ref="E153:E161"/>
-    <mergeCell ref="E134:E138"/>
-    <mergeCell ref="E104:E116"/>
-    <mergeCell ref="E54:E66"/>
-    <mergeCell ref="E212:E218"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="E46:E53"/>
-    <mergeCell ref="E127:E133"/>
+    <mergeCell ref="E67:E70"/>
+    <mergeCell ref="E139:E145"/>
     <mergeCell ref="E42:E45"/>
     <mergeCell ref="E117:E120"/>
     <mergeCell ref="E197:E204"/>
-    <mergeCell ref="E121:E126"/>
-    <mergeCell ref="A46:A53"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A85:A103"/>
+    <mergeCell ref="E134:E138"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A77:A81"/>
     <mergeCell ref="A54:A66"/>
-    <mergeCell ref="A197:A204"/>
-    <mergeCell ref="A172:A175"/>
-    <mergeCell ref="A205:A211"/>
-    <mergeCell ref="A194:A196"/>
-    <mergeCell ref="B153:B161"/>
-    <mergeCell ref="B191:B193"/>
-    <mergeCell ref="B219:B223"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A127:A133"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B187:B190"/>
+    <mergeCell ref="B212:B218"/>
     <mergeCell ref="B194:B196"/>
-    <mergeCell ref="B46:B53"/>
+    <mergeCell ref="B197:B204"/>
+    <mergeCell ref="B42:B45"/>
     <mergeCell ref="B117:B120"/>
-    <mergeCell ref="B85:B103"/>
-    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="B22:B26"/>
   </mergeCells>
   <pageMargins bottom="0.790000021457672" footer="0.19680555164814" header="0.19680555164814" left="0.790000021457672" right="0.790000021457672" top="0.790000021457672"/>
 </worksheet>

</xml_diff>